<commit_message>
GUI spectra merging started + multiple bug fixes
</commit_message>
<xml_diff>
--- a/input/spectrophotometry/dsl.4/data.input.xlsx
+++ b/input/spectrophotometry/dsl.4/data.input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\spectrophotometry\dsl.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20623741-8D0E-49AF-8D52-710DBBE74A7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB5EDD-AECB-4F6E-BC9A-803ED13B910B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="k_constants_log10" sheetId="3" r:id="rId3"/>
     <sheet name="absorbance" sheetId="4" r:id="rId4"/>
     <sheet name="mol_ext_coefficients" sheetId="5" r:id="rId5"/>
-    <sheet name="constant_names" sheetId="6" r:id="rId6"/>
+    <sheet name="target" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>wavelength</t>
+  </si>
+  <si>
+    <t>constant</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1357,15 +1360,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72735CB-A497-44A7-BD47-EF14B8B7867F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>306</v>
+      </c>
+      <c r="C2">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>